<commit_message>
display layer revisions; new USFS fire layer; legend images
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1E3BCB-7201-440A-89A3-1F680A2995BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED01AD8-7240-4CD4-8309-0354E31DD569}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
   <si>
     <t>Layer Name</t>
   </si>
@@ -401,6 +401,33 @@
   </si>
   <si>
     <t>FOA(0)</t>
+  </si>
+  <si>
+    <t>Fire Weather Forecast</t>
+  </si>
+  <si>
+    <t>https://www.wfas.net/</t>
+  </si>
+  <si>
+    <t>https://m.wfas.net/wfas_sfwp_map.html</t>
+  </si>
+  <si>
+    <t>USFS - WFAS</t>
+  </si>
+  <si>
+    <t>https://www.wfas.net/cgi-bin/mapserv?map=/var/www/html/nfdr/mapfiles/wfas_wms_new.map</t>
+  </si>
+  <si>
+    <t>today's fx: fbxday0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WFAS - daily Severe Fire Weather Potential forecast </t>
+  </si>
+  <si>
+    <t>other products avail; fx days for today &amp; tmr</t>
+  </si>
+  <si>
+    <t>https://appliedsciences.nasa.gov/system/files/docs/Jolly_WFAS_Intro.pdf</t>
   </si>
 </sst>
 </file>
@@ -478,12 +505,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -766,11 +793,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,10 +812,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="8"/>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1257,117 +1284,143 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="1"/>
+    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>107</v>
-      </c>
-      <c r="E24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
@@ -1376,8 +1429,14 @@
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1397,7 +1456,7 @@
     <hyperlink ref="H9" r:id="rId11" xr:uid="{E623C992-6AD9-41B9-804E-CBFC6693BB8D}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{365FBDD2-A0BD-43D8-8004-6257D4ADF517}"/>
     <hyperlink ref="H10" r:id="rId13" xr:uid="{8EB69032-FF7F-41B6-9AFB-EBF0DEBAC988}"/>
-    <hyperlink ref="H25" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
+    <hyperlink ref="H26" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{2079033D-1214-48DB-8317-82DC10DE2052}"/>
     <hyperlink ref="H11" r:id="rId16" xr:uid="{4D85BA65-D4C3-4CCB-ADE9-CF42A85A6E11}"/>
     <hyperlink ref="H12" r:id="rId17" xr:uid="{F0F10AA6-EA57-42A3-A0E7-4A40714B15B5}"/>
@@ -1413,13 +1472,15 @@
     <hyperlink ref="E17" r:id="rId27" xr:uid="{8CD7BBBC-181A-4AF3-B465-2C32ABDC2ABC}"/>
     <hyperlink ref="H17" r:id="rId28" xr:uid="{4EDFBC3F-5D73-428B-9AD0-125F68287643}"/>
     <hyperlink ref="E18" r:id="rId29" xr:uid="{43632C50-495C-4DD8-8666-9527D077DDC8}"/>
-    <hyperlink ref="H24" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
+    <hyperlink ref="H25" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
     <hyperlink ref="E19" r:id="rId31" xr:uid="{2253DB1F-468A-495D-B795-9472DB9A480C}"/>
     <hyperlink ref="H19" r:id="rId32" xr:uid="{310E2E0C-7476-443F-A9EC-F5D9B20A3501}"/>
     <hyperlink ref="H20" r:id="rId33" xr:uid="{CF7EE9FA-B1DD-45BA-BF44-1D0BA1A74FFF}"/>
-    <hyperlink ref="H26" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
+    <hyperlink ref="H27" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
+    <hyperlink ref="I21" r:id="rId35" xr:uid="{16CF99F9-E1B1-4C6E-A376-8F7A5016E9A3}"/>
+    <hyperlink ref="J21" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId35"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
map layer display revisions; new NWS layer tests
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED01AD8-7240-4CD4-8309-0354E31DD569}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C4C0E5-9052-4B59-93C2-CAADB20BDE14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
   <si>
     <t>Layer Name</t>
   </si>
@@ -428,6 +428,24 @@
   </si>
   <si>
     <t>https://appliedsciences.nasa.gov/system/files/docs/Jolly_WFAS_Intro.pdf</t>
+  </si>
+  <si>
+    <t>NWS Fire Hazards</t>
+  </si>
+  <si>
+    <t>https://nowcoast.noaa.gov/arcgis/rest/services/nowcoast/wwa_meteoceanhydro_longduration_hazards_time/MapServer</t>
+  </si>
+  <si>
+    <t>https://nowcoast.noaa.gov/help/#!section=updateschedule</t>
+  </si>
+  <si>
+    <t>NWS Nowcast disolved polygons - hazardous wildfire conditions</t>
+  </si>
+  <si>
+    <t>wildfire poly(39)</t>
+  </si>
+  <si>
+    <t>other products avail; dissolved polygons</t>
   </si>
 </sst>
 </file>
@@ -793,11 +811,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,117 +1334,139 @@
         <v>135</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="1"/>
+    <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>51</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>107</v>
-      </c>
-      <c r="E25" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" t="s">
-        <v>50</v>
       </c>
       <c r="E26" t="s">
         <v>53</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="E27" t="s">
         <v>53</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
@@ -1435,8 +1475,14 @@
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1456,7 +1502,7 @@
     <hyperlink ref="H9" r:id="rId11" xr:uid="{E623C992-6AD9-41B9-804E-CBFC6693BB8D}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{365FBDD2-A0BD-43D8-8004-6257D4ADF517}"/>
     <hyperlink ref="H10" r:id="rId13" xr:uid="{8EB69032-FF7F-41B6-9AFB-EBF0DEBAC988}"/>
-    <hyperlink ref="H26" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
+    <hyperlink ref="H27" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{2079033D-1214-48DB-8317-82DC10DE2052}"/>
     <hyperlink ref="H11" r:id="rId16" xr:uid="{4D85BA65-D4C3-4CCB-ADE9-CF42A85A6E11}"/>
     <hyperlink ref="H12" r:id="rId17" xr:uid="{F0F10AA6-EA57-42A3-A0E7-4A40714B15B5}"/>
@@ -1472,11 +1518,11 @@
     <hyperlink ref="E17" r:id="rId27" xr:uid="{8CD7BBBC-181A-4AF3-B465-2C32ABDC2ABC}"/>
     <hyperlink ref="H17" r:id="rId28" xr:uid="{4EDFBC3F-5D73-428B-9AD0-125F68287643}"/>
     <hyperlink ref="E18" r:id="rId29" xr:uid="{43632C50-495C-4DD8-8666-9527D077DDC8}"/>
-    <hyperlink ref="H25" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
+    <hyperlink ref="H26" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
     <hyperlink ref="E19" r:id="rId31" xr:uid="{2253DB1F-468A-495D-B795-9472DB9A480C}"/>
     <hyperlink ref="H19" r:id="rId32" xr:uid="{310E2E0C-7476-443F-A9EC-F5D9B20A3501}"/>
     <hyperlink ref="H20" r:id="rId33" xr:uid="{CF7EE9FA-B1DD-45BA-BF44-1D0BA1A74FFF}"/>
-    <hyperlink ref="H27" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
+    <hyperlink ref="H28" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
     <hyperlink ref="I21" r:id="rId35" xr:uid="{16CF99F9-E1B1-4C6E-A376-8F7A5016E9A3}"/>
     <hyperlink ref="J21" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
updates: usdm county cat count; 8wk window for Con Mon; updated SWSI; map layout revisions
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C4C0E5-9052-4B59-93C2-CAADB20BDE14}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BBCC0-4818-452B-BC0F-FFD76968D101}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="149">
   <si>
     <t>Layer Name</t>
   </si>
@@ -421,9 +421,6 @@
     <t>today's fx: fbxday0</t>
   </si>
   <si>
-    <t xml:space="preserve">WFAS - daily Severe Fire Weather Potential forecast </t>
-  </si>
-  <si>
     <t>other products avail; fx days for today &amp; tmr</t>
   </si>
   <si>
@@ -446,6 +443,30 @@
   </si>
   <si>
     <t>other products avail; dissolved polygons</t>
+  </si>
+  <si>
+    <t>NEXRAD Base Reflectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wildland Fire Assessment System - daily Severe Fire Weather Potential forecast </t>
+  </si>
+  <si>
+    <t>https://mesonet.agron.iastate.edu/ogc/</t>
+  </si>
+  <si>
+    <t>IEM</t>
+  </si>
+  <si>
+    <t>NEXRAD Base Reflectivity current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nexrad-n0q-900913	</t>
+  </si>
+  <si>
+    <t>other products avail</t>
+  </si>
+  <si>
+    <t>https://mesonet.agron.iastate.edu/cgi-bin/wms/nexrad/n0q.cgi?</t>
   </si>
 </sst>
 </file>
@@ -811,11 +832,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J31"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" sqref="A1:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1331,7 @@
         <v>127</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="C21" t="s">
         <v>130</v>
@@ -1322,7 +1346,7 @@
         <v>132</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>128</v>
@@ -1331,15 +1355,15 @@
         <v>129</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
@@ -1348,131 +1372,153 @@
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="1"/>
+      <c r="A23" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="B26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>107</v>
-      </c>
-      <c r="E26" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" t="s">
-        <v>50</v>
       </c>
       <c r="E27" t="s">
         <v>53</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="E28" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+    <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
@@ -1481,8 +1527,14 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1502,7 +1554,7 @@
     <hyperlink ref="H9" r:id="rId11" xr:uid="{E623C992-6AD9-41B9-804E-CBFC6693BB8D}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{365FBDD2-A0BD-43D8-8004-6257D4ADF517}"/>
     <hyperlink ref="H10" r:id="rId13" xr:uid="{8EB69032-FF7F-41B6-9AFB-EBF0DEBAC988}"/>
-    <hyperlink ref="H27" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
+    <hyperlink ref="H28" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{2079033D-1214-48DB-8317-82DC10DE2052}"/>
     <hyperlink ref="H11" r:id="rId16" xr:uid="{4D85BA65-D4C3-4CCB-ADE9-CF42A85A6E11}"/>
     <hyperlink ref="H12" r:id="rId17" xr:uid="{F0F10AA6-EA57-42A3-A0E7-4A40714B15B5}"/>
@@ -1518,15 +1570,16 @@
     <hyperlink ref="E17" r:id="rId27" xr:uid="{8CD7BBBC-181A-4AF3-B465-2C32ABDC2ABC}"/>
     <hyperlink ref="H17" r:id="rId28" xr:uid="{4EDFBC3F-5D73-428B-9AD0-125F68287643}"/>
     <hyperlink ref="E18" r:id="rId29" xr:uid="{43632C50-495C-4DD8-8666-9527D077DDC8}"/>
-    <hyperlink ref="H26" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
+    <hyperlink ref="H27" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
     <hyperlink ref="E19" r:id="rId31" xr:uid="{2253DB1F-468A-495D-B795-9472DB9A480C}"/>
     <hyperlink ref="H19" r:id="rId32" xr:uid="{310E2E0C-7476-443F-A9EC-F5D9B20A3501}"/>
     <hyperlink ref="H20" r:id="rId33" xr:uid="{CF7EE9FA-B1DD-45BA-BF44-1D0BA1A74FFF}"/>
-    <hyperlink ref="H28" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
+    <hyperlink ref="H29" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
     <hyperlink ref="I21" r:id="rId35" xr:uid="{16CF99F9-E1B1-4C6E-A376-8F7A5016E9A3}"/>
     <hyperlink ref="J21" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
+    <hyperlink ref="E23" r:id="rId37" xr:uid="{867A9792-BD7A-4C56-B1FF-CDD355F0DEEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId37"/>
+  <pageSetup scale="47" orientation="landscape" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix county drough legend image - case sensitive linux
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BBCC0-4818-452B-BC0F-FFD76968D101}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AE22EC-9D6D-43EB-879E-C858EF5D1625}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
   <si>
     <t>Layer Name</t>
   </si>
@@ -467,6 +467,15 @@
   </si>
   <si>
     <t>https://mesonet.agron.iastate.edu/cgi-bin/wms/nexrad/n0q.cgi?</t>
+  </si>
+  <si>
+    <t>Prev 30-day Precip</t>
+  </si>
+  <si>
+    <t>30-day total precipitation</t>
+  </si>
+  <si>
+    <t>PRECIP_TP30</t>
   </si>
 </sst>
 </file>
@@ -835,11 +844,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1278,36 +1287,33 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="C19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="C20" t="s">
         <v>119</v>
@@ -1316,215 +1322,233 @@
         <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>133</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C23" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>107</v>
-      </c>
-      <c r="E27" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
       </c>
       <c r="E28" t="s">
         <v>53</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
         <v>53</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+    <row r="30" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
@@ -1533,8 +1557,14 @@
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1554,7 +1584,7 @@
     <hyperlink ref="H9" r:id="rId11" xr:uid="{E623C992-6AD9-41B9-804E-CBFC6693BB8D}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{365FBDD2-A0BD-43D8-8004-6257D4ADF517}"/>
     <hyperlink ref="H10" r:id="rId13" xr:uid="{8EB69032-FF7F-41B6-9AFB-EBF0DEBAC988}"/>
-    <hyperlink ref="H28" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
+    <hyperlink ref="H29" r:id="rId14" xr:uid="{01A65CFE-7AEA-46AA-90E5-75C2926A652F}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{2079033D-1214-48DB-8317-82DC10DE2052}"/>
     <hyperlink ref="H11" r:id="rId16" xr:uid="{4D85BA65-D4C3-4CCB-ADE9-CF42A85A6E11}"/>
     <hyperlink ref="H12" r:id="rId17" xr:uid="{F0F10AA6-EA57-42A3-A0E7-4A40714B15B5}"/>
@@ -1570,16 +1600,17 @@
     <hyperlink ref="E17" r:id="rId27" xr:uid="{8CD7BBBC-181A-4AF3-B465-2C32ABDC2ABC}"/>
     <hyperlink ref="H17" r:id="rId28" xr:uid="{4EDFBC3F-5D73-428B-9AD0-125F68287643}"/>
     <hyperlink ref="E18" r:id="rId29" xr:uid="{43632C50-495C-4DD8-8666-9527D077DDC8}"/>
-    <hyperlink ref="H27" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
-    <hyperlink ref="E19" r:id="rId31" xr:uid="{2253DB1F-468A-495D-B795-9472DB9A480C}"/>
-    <hyperlink ref="H19" r:id="rId32" xr:uid="{310E2E0C-7476-443F-A9EC-F5D9B20A3501}"/>
-    <hyperlink ref="H20" r:id="rId33" xr:uid="{CF7EE9FA-B1DD-45BA-BF44-1D0BA1A74FFF}"/>
-    <hyperlink ref="H29" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
-    <hyperlink ref="I21" r:id="rId35" xr:uid="{16CF99F9-E1B1-4C6E-A376-8F7A5016E9A3}"/>
-    <hyperlink ref="J21" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
-    <hyperlink ref="E23" r:id="rId37" xr:uid="{867A9792-BD7A-4C56-B1FF-CDD355F0DEEA}"/>
+    <hyperlink ref="H28" r:id="rId30" xr:uid="{B24D09BB-761E-48BB-8D88-77B23B12864F}"/>
+    <hyperlink ref="E20" r:id="rId31" xr:uid="{2253DB1F-468A-495D-B795-9472DB9A480C}"/>
+    <hyperlink ref="H20" r:id="rId32" xr:uid="{310E2E0C-7476-443F-A9EC-F5D9B20A3501}"/>
+    <hyperlink ref="H21" r:id="rId33" xr:uid="{CF7EE9FA-B1DD-45BA-BF44-1D0BA1A74FFF}"/>
+    <hyperlink ref="H30" r:id="rId34" xr:uid="{65A6A7B0-E0B8-472C-8EA1-C15D7AC2AD04}"/>
+    <hyperlink ref="I22" r:id="rId35" xr:uid="{16CF99F9-E1B1-4C6E-A376-8F7A5016E9A3}"/>
+    <hyperlink ref="J22" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
+    <hyperlink ref="E24" r:id="rId37" xr:uid="{867A9792-BD7A-4C56-B1FF-CDD355F0DEEA}"/>
+    <hyperlink ref="E19" r:id="rId38" xr:uid="{412CCEAB-7397-4FA9-8E8E-3AE521BD31E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="47" orientation="landscape" verticalDpi="0" r:id="rId38"/>
+  <pageSetup scale="47" orientation="landscape" verticalDpi="0" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised app navigation with sector map displays; added statewide stats to bokeh plots
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AE22EC-9D6D-43EB-879E-C858EF5D1625}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1297F7-6990-4535-9042-812F0636EEE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="158">
   <si>
     <t>Layer Name</t>
   </si>
@@ -476,6 +476,24 @@
   </si>
   <si>
     <t>PRECIP_TP30</t>
+  </si>
+  <si>
+    <t>USDM Weeks in Drought</t>
+  </si>
+  <si>
+    <t>csv download</t>
+  </si>
+  <si>
+    <t>new REST Service available</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>REST service recently added</t>
+  </si>
+  <si>
+    <t>https://droughtmonitor.unl.edu/Data/DataDownload/WeeksInDrought.aspx</t>
   </si>
 </sst>
 </file>
@@ -847,8 +865,8 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1552,9 +1570,27 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" t="s">
+        <v>154</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
@@ -1609,8 +1645,9 @@
     <hyperlink ref="J22" r:id="rId36" xr:uid="{75A025CC-703F-499F-ACE1-89F871899D7F}"/>
     <hyperlink ref="E24" r:id="rId37" xr:uid="{867A9792-BD7A-4C56-B1FF-CDD355F0DEEA}"/>
     <hyperlink ref="E19" r:id="rId38" xr:uid="{412CCEAB-7397-4FA9-8E8E-3AE521BD31E5}"/>
+    <hyperlink ref="H31" r:id="rId39" xr:uid="{105C6714-13A4-479C-A46B-7374C3DC7479}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="47" orientation="landscape" verticalDpi="0" r:id="rId39"/>
+  <pageSetup scale="47" orientation="landscape" verticalDpi="0" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add NWM map back in nav menu
</commit_message>
<xml_diff>
--- a/map_layers_inventory.xlsx
+++ b/map_layers_inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1297F7-6990-4535-9042-812F0636EEE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D4B36-5B4B-44F9-BF51-BEB8AC64E41E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,9 +484,6 @@
     <t>csv download</t>
   </si>
   <si>
-    <t>new REST Service available</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -494,6 +491,9 @@
   </si>
   <si>
     <t>https://droughtmonitor.unl.edu/Data/DataDownload/WeeksInDrought.aspx</t>
+  </si>
+  <si>
+    <t>co_drought\workspaces\app_workspace\usdm_county_count_accum.csv</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -875,7 +875,7 @@
     <col min="2" max="2" width="44.21875" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="7" max="7" width="24.88671875" customWidth="1"/>
   </cols>
@@ -1580,16 +1580,16 @@
         <v>153</v>
       </c>
       <c r="E31" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>